<commit_message>
Final fix of the initial version
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -28,16 +28,21 @@
     <t>Result</t>
   </si>
   <si>
-    <t>2020-02-15</t>
+    <t>2020-02-19</t>
   </si>
   <si>
     <t>Test akcji</t>
   </si>
   <si>
-    <t>Passed</t>
+    <t xml:space="preserve">Failed - Message: invalid argument
+  (Session info: chrome=79.0.3945.130)
+</t>
   </si>
   <si>
     <t>Test elementow</t>
+  </si>
+  <si>
+    <t>Failed - 'NoneType' object has no attribute 'click'</t>
   </si>
 </sst>
 </file>
@@ -415,7 +420,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Simplified the code, added a class and fixed the xlsx creation
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -34,9 +34,7 @@
     <t>Test akcji</t>
   </si>
   <si>
-    <t xml:space="preserve">Failed - Message: invalid argument
-  (Session info: chrome=79.0.3945.130)
-</t>
+    <t>failed</t>
   </si>
   <si>
     <t>Test elementow</t>
@@ -63,12 +61,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -83,9 +87,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,18 +421,21 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>